<commit_message>
COMMIT COMPLETE TEST FRAMEWORK
</commit_message>
<xml_diff>
--- a/src/test/java/com/CtechInfoSys/BEAirs/TestData/BEAirsTestData.xlsx
+++ b/src/test/java/com/CtechInfoSys/BEAirs/TestData/BEAirsTestData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddNewCustomer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>PWD</t>
   </si>
@@ -36,16 +37,96 @@
   </si>
   <si>
     <t>rUzYdap</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>TelephoneNo</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>LoginPWD</t>
+  </si>
+  <si>
+    <t>LoginUID</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>A4 PRIMECITY</t>
+  </si>
+  <si>
+    <t>BANGALORE</t>
+  </si>
+  <si>
+    <t>KARNATAKA</t>
+  </si>
+  <si>
+    <t>RAJ</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>04071971</t>
+  </si>
+  <si>
+    <t>04081972</t>
+  </si>
+  <si>
+    <t>RAJAN</t>
+  </si>
+  <si>
+    <t>BAJAN</t>
+  </si>
+  <si>
+    <t>RAJ111@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>TAJ3@GMAIL.COM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,13 +149,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -355,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -385,4 +470,145 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
+        <v>560100</v>
+      </c>
+      <c r="J2">
+        <v>123456789</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3">
+        <v>560100</v>
+      </c>
+      <c r="J3">
+        <v>213456789</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>